<commit_message>
cambios en vistas y funciones
</commit_message>
<xml_diff>
--- a/Casos de prueba - Test Cases.xlsx
+++ b/Casos de prueba - Test Cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\f\Documents\ORT\Programacion 2\Obligatorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ORT\Programacion 2\Obligatorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F471F100-2E7E-4130-B442-544A2E4E37F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBCD972-0867-47A2-94A6-D849B10E9D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1ACA4504-5B2F-4E95-8B89-9627C8AFB1C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1ACA4504-5B2F-4E95-8B89-9627C8AFB1C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Caso de prueba</t>
   </si>
@@ -42,53 +42,125 @@
     <t>Resultado obtenido</t>
   </si>
   <si>
-    <t>Login exitoso de usuario administrador</t>
-  </si>
-  <si>
-    <t>1) Navegar a la pantalla de login
+    <t>Login fallido de usuario administrador</t>
+  </si>
+  <si>
+    <t>Funcionalidad</t>
+  </si>
+  <si>
+    <t>Acceder al sistema (Login)</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Captura</t>
+  </si>
+  <si>
+    <t>Login de Administrador</t>
+  </si>
+  <si>
+    <t>usuario : "marcio@example.com"
+contraseña : "marcio123"</t>
+  </si>
+  <si>
+    <t>1) Ir al link  de login en el header y hacer click login
 2) Ingresar usuario y contraseña validos
-3) Hacer click en "Login"</t>
-  </si>
-  <si>
-    <t>usuario : "admin"
-contraseña : "admin1234"</t>
-  </si>
-  <si>
-    <t>El usuario ingresa al sistema y en la barra de navegacion puede ver las opciones:
-1) Alta Propiedad
-2) Listado Barrios
-3) Logout
-4) Facturas emitidas</t>
-  </si>
-  <si>
-    <t>Login fallido de usuario administrador</t>
-  </si>
-  <si>
-    <t>1) Navegar a la pantalla de login
+3) Hacer click en "Acceder"</t>
+  </si>
+  <si>
+    <t>usuario : "marcio@example.com"
+contraseña : "marsio"</t>
+  </si>
+  <si>
+    <t>El usuario es redirigido a la misma pantalla de Login y se despliega una alerta en rojo con un error con el texto "Usuario o contraseña incorrectas"</t>
+  </si>
+  <si>
+    <t>Filtro por publicaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario ingresa al sistema y en el body puede ver:
+1) Mail con el que se logeo                                                                
+En el Header puede ver:
+1) Lista de Clientes
+2) Listado de Subastas
+3) Logout </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Navegar a la pantalla de login
 2) Ingresar usuario y contraseña invalidos
-3) Hacer click en "Login"</t>
-  </si>
-  <si>
-    <t>usuario : "admin"
-contraseña : "dumy1234"</t>
-  </si>
-  <si>
-    <t>El usuario es redirigido a la misma pantalla de Login y se despliega en rojo un error con el texto "Usuario o contraseña incorrectas"</t>
-  </si>
-  <si>
-    <t>Funcionalidad</t>
-  </si>
-  <si>
-    <t>Acceder al sistema (Login)</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Captura</t>
-  </si>
-  <si>
-    <t>Img 1</t>
+3) Hacer click en "Login"
+</t>
+  </si>
+  <si>
+    <t>1) Ir al link  de login en el header y hacer click login
+2) Ingresar usuario y contraseña validos
+3) Hacer click en "Acceder"
+4) En el headder hacer click en Publicaciones
+5) En la nueva pantalla ingresar al input de filtro
+6)Escribir "Venta" o "subasta"
+7)Click en Buscar</t>
+  </si>
+  <si>
+    <t>El usuario una vez que hace click en buscar va a poder ver la lista filtrada de venta o de subasta, es una búsqieda de acuerdo a las pubolicaciones que hay</t>
+  </si>
+  <si>
+    <t>Filtrar búsquedas</t>
+  </si>
+  <si>
+    <t>Filtro por publicaciones vacía o mal escitras</t>
+  </si>
+  <si>
+    <t>1) Ir al link  de login en el header y hacer click login
+2) Ingresar usuario y contraseña validos
+3) Hacer click en "Acceder"
+4) En el headder hacer click en Publicaciones
+5) En la nueva pantalla ingresar al input de filtro
+6)Escribir "Benta" o "Zubasta"
+7)Click en Buscar</t>
+  </si>
+  <si>
+    <t>usuario : "fede@example.com"
+contraseña : "fede123"</t>
+  </si>
+  <si>
+    <t>Al Cliente se le va a desplegar una alerta en la cual dice: "Debe ingresar un tipo de publicacion correcta o que no esté vacía"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comprar </t>
+  </si>
+  <si>
+    <t>Hacer una compra</t>
+  </si>
+  <si>
+    <t>1) Ir al link  de login en el header y hacer click login
+2) Ingresar usuario y contraseña validos
+3) Hacer click en "Acceder"
+4) En el headder hacer click en Publicaciones
+5) En la nueva pantalla ingresar al input de filtro
+6)Escribir "Venta" 
+7)Click en Buscar
+8)Seleccionar una venta y click en comprar</t>
+  </si>
+  <si>
+    <t>El cliente una vez que haya hecho la compra va a saltar un cartel que diga su compra se ha realizado con exito</t>
+  </si>
+  <si>
+    <t>Cargar Billetera</t>
+  </si>
+  <si>
+    <t>Cargar saldo en la billetera de un ususario</t>
+  </si>
+  <si>
+    <t>1) Ir al link  de login en el header y hacer click login
+2) Ingresar usuario y contraseña validos
+3) Hacer click en "Acceder"
+4) En el headder hacer click en "Billetera"
+5) Ingresar monto in input
+6)click en "Aceptar"</t>
+  </si>
+  <si>
+    <t>Luego de clickear en aceptar nos va a saltar un cartel que el monto a sido ingresado con éxito con el nombre del cliente y con el nuevo saldo. En caso de haber hecho una compra y le quedara un saldo este nuevo saldo se va a sumar al saldo que ya tenía el cliente</t>
   </si>
 </sst>
 </file>
@@ -132,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -200,51 +272,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -300,7 +327,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -316,20 +343,70 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -338,44 +415,72 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -692,92 +797,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8713D099-3472-4330-84B7-4DE559EACC68}">
-  <dimension ref="B1:H4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="55.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="55.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:8" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="15"/>
     </row>
-    <row r="3" spans="2:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="9" t="s">
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="G5" s="8"/>
     </row>
-    <row r="4" spans="2:8" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14"/>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="12"/>
+    <row r="6" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:B4"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>